<commit_message>
Refactor LLM client integration by removing custom OpenAI and Ollama clients, and introducing new provider modules for OpenAI and Ollama. Updated package dependencies to include @ai-sdk/openai and ollama-ai-provider-v2. Adjusted recorder and test executor to utilize the new provider architecture, enhancing support for local LLMs and proxy configurations.
</commit_message>
<xml_diff>
--- a/test-cases-template.xlsx
+++ b/test-cases-template.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>用例ID</t>
   </si>
@@ -85,18 +85,6 @@
   </si>
   <si>
     <t>验证跳转功能</t>
-  </si>
-  <si>
-    <t>输入用户名"longchangkun"</t>
-  </si>
-  <si>
-    <t>4.勾选我已阅读并同意复选框</t>
-  </si>
-  <si>
-    <t>5.点击"登录"按钮，跳转到（https://task-pre.renderbus.com/）</t>
-  </si>
-  <si>
-    <t>6.点击左侧导航栏的“统计”下面的 “云制作”</t>
   </si>
 </sst>
 </file>
@@ -723,13 +711,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1113,13 +1102,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
@@ -1176,7 +1165,7 @@
       <c r="B3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="3" t="s">
@@ -1187,31 +1176,11 @@
       </c>
       <c r="F3" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="D10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="D12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="D13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="D14" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" display="https://task-pre.renderbus.com/sso"/>
+    <hyperlink ref="C3" r:id="rId1" display="https://task-pre.renderbus.com/sso" tooltip="https://task-pre.renderbus.com/sso"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="portrait"/>

</xml_diff>

<commit_message>
:sparkles: Enhance AI assertion engine with new locator function and URL change handling
- Added `locatorByText` function to support text assertions in pages without `getByText`.
- Updated assertion logic to utilize the new locator function for visibility checks.
- Introduced `waitForPageLoadIfUrlChanged` method in `TestExecutor` to ensure proper page load handling after URL changes.
- Improved documentation for assertion generation and URL assertion requirements.
</commit_message>
<xml_diff>
--- a/test-cases-template.xlsx
+++ b/test-cases-template.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>用例ID</t>
   </si>
@@ -59,10 +59,11 @@
     <t>输入用户名"longchangkun"
 输入密码"Lck123456"
 勾选我已阅读并同意复选框
-点击"登录"按钮</t>
-  </si>
-  <si>
-    <t>登录成功，跳转到首页（https://task-pre.renderbus.com/）</t>
+点击"登录"按钮，跳转到 https://task-pre.renderbus.com/
+点击左侧导航栏的“统计”下面的 “云制作”</t>
+  </si>
+  <si>
+    <t>跳转成功到页面，https://task-pre.renderbus.com/desktop</t>
   </si>
   <si>
     <t>验证正常登录流程</t>
@@ -81,10 +82,10 @@
 点击左侧导航栏的“统计”下面的 “云制作”</t>
   </si>
   <si>
-    <t>跳转成功到页面，https://task-pre.renderbus.com/desktop</t>
-  </si>
-  <si>
     <t>验证跳转功能</t>
+  </si>
+  <si>
+    <t>登录成功，跳转到首页（https://task-pre.renderbus.com/）</t>
   </si>
 </sst>
 </file>
@@ -1102,13 +1103,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
@@ -1138,7 +1139,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" ht="68" spans="1:6">
+    <row r="2" ht="84" spans="1:6">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1172,9 +1173,14 @@
         <v>14</v>
       </c>
       <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
         <v>15</v>
       </c>
-      <c r="F3" t="s">
+    </row>
+    <row r="9" spans="1:6">
+      <c r="E9" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
✨ Add web assertions JSON skill and update assertion engine structure
- Introduced a new skill for generating web assertions in JSON format based on expected results and current page elements.
- Updated the assertion engine to support a simplified structure for assertions, focusing on URL and observe types.
- Removed legacy assertion types and improved documentation for assertion generation.
- Enhanced error handling and fallback mechanisms for AI assertion failures.
</commit_message>
<xml_diff>
--- a/test-cases-template.xlsx
+++ b/test-cases-template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="26860" windowHeight="13980"/>
+    <workbookView windowWidth="28260" windowHeight="13440"/>
   </bookViews>
   <sheets>
     <sheet name="测试用例" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>用例ID</t>
   </si>
@@ -54,25 +54,6 @@
   </si>
   <si>
     <t>https://task-pre.renderbus.com/sso</t>
-  </si>
-  <si>
-    <t>输入用户名"longchangkun"
-输入密码"Lck123456"
-勾选我已阅读并同意复选框
-点击"登录"按钮，跳转到 https://task-pre.renderbus.com/
-点击左侧导航栏的“统计”下面的 “云制作”</t>
-  </si>
-  <si>
-    <t>跳转成功到页面，https://task-pre.renderbus.com/desktop</t>
-  </si>
-  <si>
-    <t>验证正常登录流程</t>
-  </si>
-  <si>
-    <t>TC-002</t>
-  </si>
-  <si>
-    <t>跳转功能测试</t>
   </si>
   <si>
     <t>输入用户名"longchangkun"
@@ -82,10 +63,37 @@
 点击左侧导航栏的“统计”下面的 “云制作”</t>
   </si>
   <si>
+    <t>跳转成功到页面，https://task-pre.renderbus.com/desktop</t>
+  </si>
+  <si>
+    <t>验证正常登录流程</t>
+  </si>
+  <si>
+    <t>TC-002</t>
+  </si>
+  <si>
+    <t>跳转功能测试</t>
+  </si>
+  <si>
     <t>验证跳转功能</t>
   </si>
   <si>
     <t>登录成功，跳转到首页（https://task-pre.renderbus.com/）</t>
+  </si>
+  <si>
+    <t>输入用户名"longchangkun"</t>
+  </si>
+  <si>
+    <t>输入密码"Lck123456"</t>
+  </si>
+  <si>
+    <t>勾选我已阅读并同意复选框</t>
+  </si>
+  <si>
+    <t>点击"登录"按钮，跳转到（https://task-pre.renderbus.com/）</t>
+  </si>
+  <si>
+    <t>点击左侧导航栏的“统计”下面的 “云制作”</t>
   </si>
 </sst>
 </file>
@@ -1103,10 +1111,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="5"/>
@@ -1159,7 +1167,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" ht="84" spans="1:6">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1169,24 +1177,48 @@
       <c r="C3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>14</v>
-      </c>
+      <c r="D3" s="3"/>
       <c r="E3" t="s">
         <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="E9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4">
+      <c r="D17" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4">
+      <c r="D18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="4:4">
+      <c r="D19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="4:4">
+      <c r="D20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="4:4">
+      <c r="D21" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" display="https://task-pre.renderbus.com/sso" tooltip="https://task-pre.renderbus.com/sso"/>
+    <hyperlink ref="C2" r:id="rId1" display="https://task-pre.renderbus.com/sso"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="portrait"/>

</xml_diff>

<commit_message>
✨ Enhance data handling and assertion execution in the testing framework
- Added a new `dataStore.ts` module for managing test case data and results, including JSON serialization and file operations.
- Updated `aiAssertionEngine.ts` to allow reusing existing assertion plans, improving efficiency in verification processes.
- Modified `index.ts` to integrate data loading and result saving functionalities, streamlining the test execution workflow.
- Enhanced `TestExecutor` to support recorded actions and assertion plans, enabling more efficient test case execution.
- Improved error handling and logging throughout the testing process for better diagnostics.
- Updated `.gitignore` to include the new `data/` directory for generated files.
</commit_message>
<xml_diff>
--- a/test-cases-template.xlsx
+++ b/test-cases-template.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>用例ID</t>
   </si>
@@ -54,25 +54,35 @@
   </si>
   <si>
     <t>https://task-pre.renderbus.com/sso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">输入用户名"longchangkun"
+输入密码"Lck123456"
+勾选我已阅读并同意复选框
+点击"登录"按钮
+</t>
+  </si>
+  <si>
+    <t>跳转成功到页面，https://task-pre.renderbus.com/</t>
+  </si>
+  <si>
+    <t>验证正常登录流程</t>
+  </si>
+  <si>
+    <t>TC-002</t>
+  </si>
+  <si>
+    <t>跳转功能测试</t>
   </si>
   <si>
     <t>输入用户名"longchangkun"
 输入密码"Lck123456"
 勾选我已阅读并同意复选框
-点击"登录"按钮，跳转到（https://task-pre.renderbus.com/）
+点击"登录"按钮
 点击左侧导航栏的“统计”下面的 “云制作”</t>
   </si>
   <si>
     <t>跳转成功到页面，https://task-pre.renderbus.com/desktop</t>
-  </si>
-  <si>
-    <t>验证正常登录流程</t>
-  </si>
-  <si>
-    <t>TC-002</t>
-  </si>
-  <si>
-    <t>跳转功能测试</t>
   </si>
   <si>
     <t>验证跳转功能</t>
@@ -1114,7 +1124,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="5"/>
@@ -1167,7 +1177,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" ht="84" spans="1:6">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1177,42 +1187,44 @@
       <c r="C3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="3"/>
+      <c r="D3" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="E9" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="4:4">
       <c r="D17" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="4:4">
       <c r="D18" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="4:4">
       <c r="D19" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="4:4">
       <c r="D20" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="4:4">
       <c r="D21" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
✨ Update test execution and data handling features
- Added support for Playwright trace recording, including options for trace directory and recording control in `TestExecutor`.
- Removed deprecated `skipPageLoadWait` field from `TestResultJson` to streamline data structure.
- Updated `.gitignore` to include `traces/` directory for generated trace files.
- Enhanced `TestExecutor` with improved page load handling and error diagnostics during test execution.
</commit_message>
<xml_diff>
--- a/test-cases-template.xlsx
+++ b/test-cases-template.xlsx
@@ -75,20 +75,20 @@
     <t>跳转功能测试</t>
   </si>
   <si>
+    <t>跳转成功到页面，https://task-pre.renderbus.com/desktop</t>
+  </si>
+  <si>
+    <t>验证跳转功能</t>
+  </si>
+  <si>
+    <t>登录成功，跳转到首页（https://task-pre.renderbus.com/）</t>
+  </si>
+  <si>
     <t>输入用户名"longchangkun"
 输入密码"Lck123456"
 勾选我已阅读并同意复选框
 点击"登录"按钮
 点击左侧导航栏的“统计”下面的 “云制作”</t>
-  </si>
-  <si>
-    <t>跳转成功到页面，https://task-pre.renderbus.com/desktop</t>
-  </si>
-  <si>
-    <t>验证跳转功能</t>
-  </si>
-  <si>
-    <t>登录成功，跳转到首页（https://task-pre.renderbus.com/）</t>
   </si>
   <si>
     <t>输入用户名"longchangkun"</t>
@@ -730,7 +730,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
@@ -738,6 +738,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1124,7 +1127,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="5"/>
@@ -1177,7 +1180,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" ht="84" spans="1:6">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1187,18 +1190,21 @@
       <c r="C3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="3"/>
+      <c r="E3" t="s">
         <v>14</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>15</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="E9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" ht="84" spans="1:6">
+      <c r="D10" s="5" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
✨ Update test execution timeout and enhance trace recording
- Reduced default timeout in `TestExecutor` from 30 seconds to 5 seconds for quicker test execution.
- Modified URL change handling to ensure `timedOut` is always set to true when the URL remains unchanged.
- Added a wait for network idle before stopping trace recording to ensure all requests are captured, improving trace accuracy.
- Updated the test cases template file to reflect recent changes.
</commit_message>
<xml_diff>
--- a/test-cases-template.xlsx
+++ b/test-cases-template.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>用例ID</t>
   </si>
@@ -54,34 +54,6 @@
   </si>
   <si>
     <t>https://task-pre.renderbus.com/sso</t>
-  </si>
-  <si>
-    <t xml:space="preserve">输入用户名"longchangkun"
-输入密码"Lck123456"
-勾选我已阅读并同意复选框
-点击"登录"按钮
-</t>
-  </si>
-  <si>
-    <t>跳转成功到页面，https://task-pre.renderbus.com/</t>
-  </si>
-  <si>
-    <t>验证正常登录流程</t>
-  </si>
-  <si>
-    <t>TC-002</t>
-  </si>
-  <si>
-    <t>跳转功能测试</t>
-  </si>
-  <si>
-    <t>跳转成功到页面，https://task-pre.renderbus.com/desktop</t>
-  </si>
-  <si>
-    <t>验证跳转功能</t>
-  </si>
-  <si>
-    <t>登录成功，跳转到首页（https://task-pre.renderbus.com/）</t>
   </si>
   <si>
     <t>输入用户名"longchangkun"
@@ -91,19 +63,31 @@
 点击左侧导航栏的“统计”下面的 “云制作”</t>
   </si>
   <si>
-    <t>输入用户名"longchangkun"</t>
-  </si>
-  <si>
-    <t>输入密码"Lck123456"</t>
-  </si>
-  <si>
-    <t>勾选我已阅读并同意复选框</t>
-  </si>
-  <si>
-    <t>点击"登录"按钮，跳转到（https://task-pre.renderbus.com/）</t>
-  </si>
-  <si>
-    <t>点击左侧导航栏的“统计”下面的 “云制作”</t>
+    <t>跳转成功到页面，https://task-pre.renderbus.com/desktop</t>
+  </si>
+  <si>
+    <t>验证正常登录流程</t>
+  </si>
+  <si>
+    <t>TC-002</t>
+  </si>
+  <si>
+    <t>跳转功能测试</t>
+  </si>
+  <si>
+    <t>验证跳转功能</t>
+  </si>
+  <si>
+    <t>登录成功，跳转到首页（https://task-pre.renderbus.com/）</t>
+  </si>
+  <si>
+    <t>输入用户名"longchangkun"
+输入密码"Lck123456"
+勾选我已阅读并同意复选框
+点击"登录"按钮</t>
+  </si>
+  <si>
+    <t>跳转成功到页面，https://task-pre.renderbus.com/</t>
   </si>
 </sst>
 </file>
@@ -1124,10 +1108,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="5"/>
@@ -1192,45 +1176,28 @@
       </c>
       <c r="D3" s="3"/>
       <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
         <v>14</v>
-      </c>
-      <c r="F3" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="E9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" ht="84" spans="1:6">
       <c r="D10" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" ht="68" spans="1:6">
+      <c r="D13" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="4:4">
-      <c r="D17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="4:4">
-      <c r="D18" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="4:4">
-      <c r="D19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="4:4">
-      <c r="D20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="4:4">
-      <c r="D21" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>